<commit_message>
Scores added to dataframe and saved to xlsx
</commit_message>
<xml_diff>
--- a/Odds-Data-Clean/2019-20.xlsx
+++ b/Odds-Data-Clean/2019-20.xlsx
@@ -424,12 +424,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Toronto Raptors</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -466,12 +466,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>LALakers</t>
+          <t>Los Angeles Lakers</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -508,12 +508,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Indiana Pacers</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Detroit Pistons</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -550,12 +550,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orlando Magic</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -592,12 +592,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -634,12 +634,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -676,12 +676,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami Heat</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Memphis Grizzlies</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -716,14 +716,10 @@
           <t>2019-20-1023</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -760,12 +756,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -802,12 +798,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Washington Wizards</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -844,14 +840,10 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Utah</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+          <t>Utah Jazz</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
         <v>222</v>
       </c>
@@ -886,12 +878,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Phoenix Suns</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -928,12 +920,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Nuggets</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -970,12 +962,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Detroit Pistons</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -1012,12 +1004,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -1054,12 +1046,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -1096,12 +1088,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Toronto Raptors</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -1138,12 +1130,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -1178,14 +1170,10 @@
           <t>2019-20-1025</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1220,14 +1208,10 @@
           <t>2019-20-1025</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Washington Wizards</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1264,12 +1248,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1306,12 +1290,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Memphis Grizzlies</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1348,12 +1332,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Nuggets</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Phoenix Suns</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -1390,12 +1374,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1432,12 +1416,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LALakers</t>
+          <t>Los Angeles Lakers</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Utah Jazz</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1474,12 +1458,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami Heat</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1516,12 +1500,12 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Detroit Pistons</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1558,12 +1542,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1600,12 +1584,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orlando Magic</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1642,12 +1626,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Indiana Pacers</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1684,12 +1668,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Toronto Raptors</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1726,12 +1710,12 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1768,12 +1752,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Washington Wizards</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1810,12 +1794,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Utah Jazz</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1852,12 +1836,12 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Phoenix Suns</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1892,14 +1876,10 @@
           <t>2019-20-1027</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+      <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1936,14 +1916,10 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Memphis</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+          <t>Memphis Grizzlies</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr"/>
       <c r="E38" t="n">
         <v>224</v>
       </c>
@@ -1978,12 +1954,12 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami Heat</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -2020,12 +1996,12 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -2062,12 +2038,12 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>LALakers</t>
+          <t>Los Angeles Lakers</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -2104,12 +2080,12 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Detroit Pistons</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Indiana Pacers</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -2146,12 +2122,12 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -2188,12 +2164,12 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -2230,12 +2206,12 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Toronto Raptors</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orlando Magic</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -2272,12 +2248,12 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -2314,12 +2290,12 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -2356,14 +2332,10 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Houston</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+          <t>Houston Rockets</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr"/>
       <c r="E48" t="n">
         <v>225</v>
       </c>
@@ -2398,12 +2370,12 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -2440,12 +2412,12 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Phoenix Suns</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Utah Jazz</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -2482,12 +2454,12 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Nuggets</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -2524,12 +2496,12 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -2566,12 +2538,12 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami Heat</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -2608,12 +2580,12 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Nuggets</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -2650,12 +2622,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>LALakers</t>
+          <t>Los Angeles Lakers</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Memphis Grizzlies</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -2692,12 +2664,12 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orlando Magic</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -2734,12 +2706,12 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="E57" t="n">
@@ -2776,12 +2748,12 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -2818,12 +2790,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Toronto Raptors</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Detroit Pistons</t>
         </is>
       </c>
       <c r="E59" t="n">
@@ -2858,14 +2830,10 @@
           <t>2019-20-1030</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+      <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Indiana Pacers</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -2902,12 +2870,12 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="E61" t="n">
@@ -2944,12 +2912,12 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Washington Wizards</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -2984,14 +2952,10 @@
           <t>2019-20-1030</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+      <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="E63" t="n">
@@ -3028,12 +2992,12 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="E64" t="n">
@@ -3070,12 +3034,12 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Utah Jazz</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="E65" t="n">
@@ -3112,12 +3076,12 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Phoenix Suns</t>
         </is>
       </c>
       <c r="E66" t="n">
@@ -3154,12 +3118,12 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami Heat</t>
         </is>
       </c>
       <c r="E67" t="n">
@@ -3196,12 +3160,12 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Nuggets</t>
         </is>
       </c>
       <c r="E68" t="n">
@@ -3238,12 +3202,12 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="E69" t="n">
@@ -3278,14 +3242,10 @@
           <t>2019-20-1101</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+      <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="E70" t="n">
@@ -3322,12 +3282,12 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orlando Magic</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="E71" t="n">
@@ -3364,12 +3324,12 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Indiana Pacers</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="E72" t="n">
@@ -3406,12 +3366,12 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="E73" t="n">
@@ -3448,12 +3408,12 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Detroit Pistons</t>
         </is>
       </c>
       <c r="E74" t="n">
@@ -3490,12 +3450,12 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>LALakers</t>
+          <t>Los Angeles Lakers</t>
         </is>
       </c>
       <c r="E75" t="n">
@@ -3532,12 +3492,12 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Utah Jazz</t>
         </is>
       </c>
       <c r="E76" t="n">
@@ -3574,12 +3534,12 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="E77" t="n">
@@ -3614,14 +3574,10 @@
           <t>2019-20-1102</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+      <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="E78" t="n">
@@ -3658,14 +3614,10 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Detroit</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+          <t>Detroit Pistons</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr"/>
       <c r="E79" t="n">
         <v>224</v>
       </c>
@@ -3700,12 +3652,12 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orlando Magic</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Nuggets</t>
         </is>
       </c>
       <c r="E80" t="n">
@@ -3742,12 +3694,12 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Memphis Grizzlies</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Phoenix Suns</t>
         </is>
       </c>
       <c r="E81" t="n">
@@ -3784,12 +3736,12 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Washington Wizards</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="E82" t="n">
@@ -3826,12 +3778,12 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Toronto Raptors</t>
         </is>
       </c>
       <c r="E83" t="n">
@@ -3868,12 +3820,12 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="E84" t="n">
@@ -3910,12 +3862,12 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -3952,12 +3904,12 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Indiana Pacers</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="E86" t="n">
@@ -3994,12 +3946,12 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami Heat</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="E87" t="n">
@@ -4036,12 +3988,12 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="E88" t="n">
@@ -4078,12 +4030,12 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>LALakers</t>
+          <t>Los Angeles Lakers</t>
         </is>
       </c>
       <c r="E89" t="n">
@@ -4120,12 +4072,12 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="E90" t="n">
@@ -4162,12 +4114,12 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Utah Jazz</t>
         </is>
       </c>
       <c r="E91" t="n">
@@ -4204,12 +4156,12 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Washington Wizards</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Detroit Pistons</t>
         </is>
       </c>
       <c r="E92" t="n">
@@ -4244,14 +4196,10 @@
           <t>2019-20-1104</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+      <c r="C93" t="inlineStr"/>
       <c r="D93" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="E93" t="n">
@@ -4288,12 +4236,12 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="E94" t="n">
@@ -4330,12 +4278,12 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Memphis Grizzlies</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="E95" t="n">
@@ -4372,12 +4320,12 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Phoenix Suns</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="E96" t="n">
@@ -4414,12 +4362,12 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="E97" t="n">
@@ -4456,12 +4404,12 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="E98" t="n">
@@ -4498,12 +4446,12 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Indiana Pacers</t>
         </is>
       </c>
       <c r="E99" t="n">
@@ -4540,12 +4488,12 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="E100" t="n">
@@ -4580,14 +4528,10 @@
           <t>2019-20-1105</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+      <c r="C101" t="inlineStr"/>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orlando Magic</t>
         </is>
       </c>
       <c r="E101" t="n">
@@ -4624,12 +4568,12 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>LALakers</t>
+          <t>Los Angeles Lakers</t>
         </is>
       </c>
       <c r="E102" t="n">
@@ -4666,12 +4610,12 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Nuggets</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami Heat</t>
         </is>
       </c>
       <c r="E103" t="n">
@@ -4708,12 +4652,12 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Detroit Pistons</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="E104" t="n">
@@ -4750,12 +4694,12 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Indiana Pacers</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Washington Wizards</t>
         </is>
       </c>
       <c r="E105" t="n">
@@ -4792,12 +4736,12 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Toronto Raptors</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="E106" t="n">
@@ -4834,12 +4778,12 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="E107" t="n">
@@ -4876,12 +4820,12 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="E108" t="n">
@@ -4918,12 +4862,12 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Memphis Grizzlies</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="E109" t="n">
@@ -4960,12 +4904,12 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orlando Magic</t>
         </is>
       </c>
       <c r="E110" t="n">
@@ -5002,12 +4946,12 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Utah Jazz</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="E111" t="n">
@@ -5044,12 +4988,12 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="E112" t="n">
@@ -5086,12 +5030,12 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="E113" t="n">
@@ -5128,14 +5072,10 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+          <t>San Antonio Spurs</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr"/>
       <c r="E114" t="n">
         <v>214.5</v>
       </c>
@@ -5170,12 +5110,12 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Phoenix Suns</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami Heat</t>
         </is>
       </c>
       <c r="E115" t="n">
@@ -5212,12 +5152,12 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="E116" t="n">
@@ -5254,12 +5194,12 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Indiana Pacers</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Detroit Pistons</t>
         </is>
       </c>
       <c r="E117" t="n">
@@ -5296,12 +5236,12 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Washington Wizards</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="E118" t="n">
@@ -5338,12 +5278,12 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orlando Magic</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Memphis Grizzlies</t>
         </is>
       </c>
       <c r="E119" t="n">
@@ -5380,12 +5320,12 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="E120" t="n">
@@ -5422,12 +5362,12 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="E121" t="n">
@@ -5464,12 +5404,12 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Toronto Raptors</t>
         </is>
       </c>
       <c r="E122" t="n">
@@ -5506,12 +5446,12 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="E123" t="n">
@@ -5548,12 +5488,12 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Utah Jazz</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="E124" t="n">
@@ -5590,12 +5530,12 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Nuggets</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="E125" t="n">
@@ -5632,14 +5572,10 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Portland</t>
-        </is>
-      </c>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+          <t>Portland Trail Blazers</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr"/>
       <c r="E126" t="n">
         <v>233</v>
       </c>
@@ -5674,12 +5610,12 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>LALakers</t>
+          <t>Los Angeles Lakers</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami Heat</t>
         </is>
       </c>
       <c r="E127" t="n">
@@ -5716,12 +5652,12 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="E128" t="n">
@@ -5758,12 +5694,12 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="E129" t="n">
@@ -5798,14 +5734,10 @@
           <t>2019-20-1109</t>
         </is>
       </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+      <c r="C130" t="inlineStr"/>
       <c r="D130" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="E130" t="n">
@@ -5842,12 +5774,12 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Memphis Grizzlies</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="E131" t="n">
@@ -5884,12 +5816,12 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="E132" t="n">
@@ -5926,12 +5858,12 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Nuggets</t>
         </is>
       </c>
       <c r="E133" t="n">
@@ -5968,12 +5900,12 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orlando Magic</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Indiana Pacers</t>
         </is>
       </c>
       <c r="E134" t="n">
@@ -6010,12 +5942,12 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="E135" t="n">
@@ -6050,14 +5982,10 @@
           <t>2019-20-1110</t>
         </is>
       </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+      <c r="C136" t="inlineStr"/>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="E136" t="n">
@@ -6094,12 +6022,12 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="E137" t="n">
@@ -6136,14 +6064,10 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Phoenix</t>
-        </is>
-      </c>
-      <c r="D138" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+          <t>Phoenix Suns</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr"/>
       <c r="E138" t="n">
         <v>233</v>
       </c>
@@ -6178,12 +6102,12 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="E139" t="n">
@@ -6220,12 +6144,12 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>LALakers</t>
+          <t>Los Angeles Lakers</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Toronto Raptors</t>
         </is>
       </c>
       <c r="E140" t="n">
@@ -6262,12 +6186,12 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Detroit Pistons</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="E141" t="n">
@@ -6304,12 +6228,12 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="E142" t="n">
@@ -6346,12 +6270,12 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Memphis Grizzlies</t>
         </is>
       </c>
       <c r="E143" t="n">
@@ -6388,12 +6312,12 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="E144" t="n">
@@ -6430,12 +6354,12 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Utah Jazz</t>
         </is>
       </c>
       <c r="E145" t="n">
@@ -6472,12 +6396,12 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Toronto Raptors</t>
         </is>
       </c>
       <c r="E146" t="n">
@@ -6514,12 +6438,12 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="E147" t="n">
@@ -6556,14 +6480,10 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Indiana</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+          <t>Indiana Pacers</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr"/>
       <c r="E148" t="n">
         <v>209.5</v>
       </c>
@@ -6598,12 +6518,12 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami Heat</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Detroit Pistons</t>
         </is>
       </c>
       <c r="E149" t="n">
@@ -6640,12 +6560,12 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="E150" t="n">
@@ -6682,12 +6602,12 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Phoenix Suns</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>LALakers</t>
+          <t>Los Angeles Lakers</t>
         </is>
       </c>
       <c r="E151" t="n">
@@ -6724,12 +6644,12 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Nuggets</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="E152" t="n">
@@ -6766,14 +6686,10 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Utah</t>
-        </is>
-      </c>
-      <c r="D153" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+          <t>Utah Jazz</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr"/>
       <c r="E153" t="n">
         <v>217</v>
       </c>
@@ -6808,12 +6724,12 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="E154" t="n">
@@ -6850,12 +6766,12 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orlando Magic</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="E155" t="n">
@@ -6892,12 +6808,12 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Memphis Grizzlies</t>
         </is>
       </c>
       <c r="E156" t="n">
@@ -6934,12 +6850,12 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="E157" t="n">
@@ -6976,12 +6892,12 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Washington Wizards</t>
         </is>
       </c>
       <c r="E158" t="n">
@@ -7018,12 +6934,12 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="E159" t="n">
@@ -7060,12 +6976,12 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Toronto Raptors</t>
         </is>
       </c>
       <c r="E160" t="n">
@@ -7102,12 +7018,12 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>LALakers</t>
+          <t>Los Angeles Lakers</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="E161" t="n">
@@ -7144,12 +7060,12 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami Heat</t>
         </is>
       </c>
       <c r="E162" t="n">
@@ -7186,12 +7102,12 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="E163" t="n">
@@ -7228,12 +7144,12 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="E164" t="n">
@@ -7270,12 +7186,12 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="E165" t="n">
@@ -7312,12 +7228,12 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Phoenix Suns</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="E166" t="n">
@@ -7354,14 +7270,10 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Denver</t>
-        </is>
-      </c>
-      <c r="D167" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+          <t>Denver Nuggets</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr"/>
       <c r="E167" t="n">
         <v>225.5</v>
       </c>
@@ -7396,12 +7308,12 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Detroit Pistons</t>
         </is>
       </c>
       <c r="E168" t="n">
@@ -7438,12 +7350,12 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orlando Magic</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="E169" t="n">
@@ -7480,12 +7392,12 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Washington Wizards</t>
         </is>
       </c>
       <c r="E170" t="n">
@@ -7522,12 +7434,12 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Indiana Pacers</t>
         </is>
       </c>
       <c r="E171" t="n">
@@ -7562,14 +7474,10 @@
           <t>2019-20-1115</t>
         </is>
       </c>
-      <c r="C172" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+      <c r="C172" t="inlineStr"/>
       <c r="D172" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="E172" t="n">
@@ -7606,12 +7514,12 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Memphis Grizzlies</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Utah Jazz</t>
         </is>
       </c>
       <c r="E173" t="n">
@@ -7648,12 +7556,12 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="E174" t="n">
@@ -7690,12 +7598,12 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>LALakers</t>
+          <t>Los Angeles Lakers</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="E175" t="n">
@@ -7732,14 +7640,10 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Chicago</t>
-        </is>
-      </c>
-      <c r="D176" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+          <t>Chicago Bulls</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr"/>
       <c r="E176" t="n">
         <v>231.5</v>
       </c>
@@ -7774,12 +7678,12 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Indiana Pacers</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="E177" t="n">
@@ -7816,12 +7720,12 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="E178" t="n">
@@ -7858,12 +7762,12 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="E179" t="n">
@@ -7900,12 +7804,12 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami Heat</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="E180" t="n">
@@ -7942,12 +7846,12 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Toronto Raptors</t>
         </is>
       </c>
       <c r="E181" t="n">
@@ -7984,12 +7888,12 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="E182" t="n">
@@ -8026,12 +7930,12 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="E183" t="n">
@@ -8068,12 +7972,12 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="E184" t="n">
@@ -8110,12 +8014,12 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="E185" t="n">
@@ -8152,12 +8056,12 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Memphis Grizzlies</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Nuggets</t>
         </is>
       </c>
       <c r="E186" t="n">
@@ -8194,12 +8098,12 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orlando Magic</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Washington Wizards</t>
         </is>
       </c>
       <c r="E187" t="n">
@@ -8236,12 +8140,12 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="E188" t="n">
@@ -8278,12 +8182,12 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>LALakers</t>
+          <t>Los Angeles Lakers</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="E189" t="n">
@@ -8320,12 +8224,12 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="E190" t="n">
@@ -8360,14 +8264,10 @@
           <t>2019-20-1118</t>
         </is>
       </c>
-      <c r="C191" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+      <c r="C191" t="inlineStr"/>
       <c r="D191" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Indiana Pacers</t>
         </is>
       </c>
       <c r="E191" t="n">
@@ -8404,12 +8304,12 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Toronto Raptors</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="E192" t="n">
@@ -8446,12 +8346,12 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="E193" t="n">
@@ -8488,12 +8388,12 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="E194" t="n">
@@ -8530,12 +8430,12 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="E195" t="n">
@@ -8572,12 +8472,12 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Utah Jazz</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="E196" t="n">
@@ -8614,12 +8514,12 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Phoenix Suns</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="E197" t="n">
@@ -8656,14 +8556,10 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>LAClippers</t>
-        </is>
-      </c>
-      <c r="D198" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+          <t>Los Angeles Clippers</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr"/>
       <c r="E198" t="n">
         <v>219.5</v>
       </c>
@@ -8698,12 +8594,12 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="E199" t="n">
@@ -8740,12 +8636,12 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Memphis Grizzlies</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="E200" t="n">
@@ -8782,12 +8678,12 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Phoenix Suns</t>
         </is>
       </c>
       <c r="E201" t="n">
@@ -8824,14 +8720,10 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>LALakers</t>
-        </is>
-      </c>
-      <c r="D202" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+          <t>Los Angeles Lakers</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr"/>
       <c r="E202" t="n">
         <v>210.5</v>
       </c>
@@ -8866,12 +8758,12 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>NewYork</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="E203" t="n">
@@ -8908,12 +8800,12 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Washington Wizards</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="E204" t="n">
@@ -8950,12 +8842,12 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami Heat</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="E205" t="n">
@@ -8992,12 +8884,12 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="E206" t="n">
@@ -9034,12 +8926,12 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="E207" t="n">
@@ -9074,14 +8966,10 @@
           <t>2019-20-1120</t>
         </is>
       </c>
-      <c r="C208" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+      <c r="C208" t="inlineStr"/>
       <c r="D208" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="E208" t="n">
@@ -9118,12 +9006,12 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Toronto Raptors</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Orlando Magic</t>
         </is>
       </c>
       <c r="E209" t="n">
@@ -9160,12 +9048,12 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Detroit Pistons</t>
         </is>
       </c>
       <c r="E210" t="n">
@@ -9202,12 +9090,12 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Minnesota Timberwolves</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Utah Jazz</t>
         </is>
       </c>
       <c r="E211" t="n">
@@ -9244,12 +9132,12 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Nuggets</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="E212" t="n">
@@ -9286,12 +9174,12 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="E213" t="n">
@@ -9328,12 +9216,12 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Portland Trail Blazers</t>
         </is>
       </c>
       <c r="E214" t="n">
@@ -9370,12 +9258,12 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Phoenix Suns</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>NewOrleans</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="E215" t="n">
@@ -9412,12 +9300,12 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Detroit Pistons</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Atlanta Hawks</t>
         </is>
       </c>
       <c r="E216" t="n">
@@ -9454,12 +9342,12 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Washington Wizards</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Charlotte Bobcats</t>
         </is>
       </c>
       <c r="E217" t="n">
@@ -9494,14 +9382,10 @@
           <t>2019-20-1122</t>
         </is>
       </c>
-      <c r="C218" t="inlineStr">
-        <is>
-          <t>Brooklyn</t>
-        </is>
-      </c>
+      <c r="C218" t="inlineStr"/>
       <c r="D218" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Sacramento Kings</t>
         </is>
       </c>
       <c r="E218" t="n">
@@ -9538,12 +9422,12 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>SanAntonio</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="E219" t="n">
@@ -9580,12 +9464,12 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Chicago Bulls</t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami Heat</t>
         </is>
       </c>
       <c r="E220" t="n">
@@ -9620,14 +9504,10 @@
           <t>2019-20-1122</t>
         </is>
       </c>
-      <c r="C221" t="inlineStr">
-        <is>
-          <t>OklahomaCity</t>
-        </is>
-      </c>
+      <c r="C221" t="inlineStr"/>
       <c r="D221" t="inlineStr">
         <is>
-          <t>LALakers</t>
+          <t>Los Angeles Lakers</t>
         </is>
       </c>
       <c r="E221" t="n">
@@ -9664,12 +9544,12 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Cleveland Cavaliers</t>
         </is>
       </c>
       <c r="E222" t="n">
@@ -9706,12 +9586,12 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Nuggets</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="E223" t="n">
@@ -9748,12 +9628,12 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Utah Jazz</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>GoldenState</t>
+          <t>Golden State Warriors</t>
         </is>
       </c>
       <c r="E224" t="n">
@@ -9790,12 +9670,12 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>LAClippers</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Houston Rockets</t>
         </is>
       </c>
       <c r="E225" t="n">

</xml_diff>